<commit_message>
Mexico population 2010 und 2020!!!
</commit_message>
<xml_diff>
--- a/excel/Cap3/Tabla Mortalidad con Arriaga_Ejemplo.xlsx
+++ b/excel/Cap3/Tabla Mortalidad con Arriaga_Ejemplo.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://redescolmex-my.sharepoint.com/personal/agpena_colmex_mx/Documents/DEP_22_26/6to semestre/UNAM/Evaluaciones/LT/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://redescolmex-my.sharepoint.com/personal/agpena_colmex_mx/Documents/DEP_22_26/6to semestre/UNAM/test/ciencias_unam_2025-2/excel/Cap3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="24" documentId="8_{C31DF124-F43A-4C4F-9F77-BB3CE07E5119}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4B7D0688-A843-477C-80C5-DCF0267BC138}"/>
+  <xr:revisionPtr revIDLastSave="45" documentId="8_{C31DF124-F43A-4C4F-9F77-BB3CE07E5119}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6B8D0C91-D732-4610-8A9C-EBEDF8785AE0}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="781" activeTab="3" xr2:uid="{AA1FD95C-5C7D-4022-A558-3323BFE15373}"/>
   </bookViews>
@@ -983,7 +983,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1336,8 +1336,8 @@
       <xdr:rowOff>51435</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="518219" cy="175369"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2" name="TextBox 1">
@@ -1433,7 +1433,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2" name="TextBox 1">
@@ -2460,7 +2460,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0650E363-E2C5-417C-A0D3-41941F45D018}">
   <dimension ref="A1:O22"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -2552,40 +2554,39 @@
       <c r="D4" s="11">
         <v>6684</v>
       </c>
-      <c r="E4" s="12">
-        <f>D4/C4</f>
-        <v>3.6853451840742804E-2</v>
+      <c r="E4" s="32">
+        <f ca="1">J4/K4</f>
+        <v>4.5645260778884852E-2</v>
       </c>
       <c r="F4" s="17">
-        <f>IF($E$4&gt;=0.107, 0.35, 0.053+2.8*$E$4)</f>
-        <v>0.15618966515407984</v>
-      </c>
-      <c r="G4" s="12">
-        <f t="shared" ref="G4:G11" si="0">(B4*E4)/(1+(B4-F4)*E4)</f>
-        <v>3.574197216833902E-2</v>
+        <f ca="1">IF($E$4&gt;=0.107, 0.35, 0.053+2.8*$E$4)</f>
+        <v>0.18080673018087756</v>
+      </c>
+      <c r="G4" s="32">
+        <v>4.3999999999999997E-2</v>
       </c>
       <c r="H4" s="12">
         <f>1-G4</f>
-        <v>0.96425802783166104</v>
+        <v>0.95599999999999996</v>
       </c>
       <c r="I4" s="14">
         <v>100000</v>
       </c>
       <c r="J4" s="14">
-        <f t="shared" ref="J4:J12" si="1">I4-I5</f>
-        <v>3574.197216833898</v>
+        <f t="shared" ref="J4:J12" si="0">I4-I5</f>
+        <v>4400</v>
       </c>
       <c r="K4" s="14">
-        <f t="shared" ref="K4:K13" si="2">(B4*I5)+(F4*J4)</f>
-        <v>96984.05544965803</v>
+        <f t="shared" ref="K4:K13" ca="1" si="1">(B4*I5)+(F4*J4)</f>
+        <v>96395.549612795861</v>
       </c>
       <c r="L4" s="14">
-        <f>L5+K4</f>
-        <v>6973898.5814585518</v>
+        <f ca="1">L5+K4</f>
+        <v>6914398.1836870424</v>
       </c>
       <c r="M4" s="18">
-        <f t="shared" ref="M4:M22" si="3">L4/I4</f>
-        <v>69.738985814585519</v>
+        <f t="shared" ref="M4:M22" ca="1" si="2">L4/I4</f>
+        <v>69.143981836870424</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.3">
@@ -2606,36 +2607,36 @@
         <v>5.6623841486438077E-3</v>
       </c>
       <c r="F5" s="13">
-        <f>IF($E$4&gt;=0.107, 1.361, 1.522-1.518*$E$4)</f>
-        <v>1.4660564601057524</v>
+        <f ca="1">IF($E$4&gt;=0.107, 1.361, 1.522-1.518*$E$4)</f>
+        <v>1.4527104941376527</v>
       </c>
       <c r="G5" s="12">
-        <f t="shared" si="0"/>
-        <v>2.2329154277619726E-2</v>
+        <f t="shared" ref="G4:G11" ca="1" si="3">(B5*E5)/(1+(B5-F5)*E5)</f>
+        <v>2.2327490856480562E-2</v>
       </c>
       <c r="H5" s="12">
-        <f>1-G5</f>
-        <v>0.97767084572238028</v>
+        <f ca="1">1-G5</f>
+        <v>0.97767250914351944</v>
       </c>
       <c r="I5" s="14">
         <f t="shared" ref="I5:I15" si="4">I4*H4</f>
-        <v>96425.802783166102</v>
+        <v>95600</v>
       </c>
       <c r="J5" s="14">
-        <f t="shared" si="1"/>
-        <v>2153.1066266886482</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>2134.5081258795399</v>
       </c>
       <c r="K5" s="14">
-        <f t="shared" si="2"/>
-        <v>380247.3605052632</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>376962.78985076916</v>
       </c>
       <c r="L5" s="14">
-        <f>L6+K5</f>
-        <v>6876914.5260088937</v>
+        <f ca="1">L6+K5</f>
+        <v>6818002.6340742465</v>
       </c>
       <c r="M5" s="15">
-        <f t="shared" si="3"/>
-        <v>71.318198319521343</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>71.318019184877059</v>
       </c>
       <c r="O5" s="4"/>
     </row>
@@ -2661,7 +2662,7 @@
         <v>2.5</v>
       </c>
       <c r="G6" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>4.4853720803031119E-3</v>
       </c>
       <c r="H6" s="12">
@@ -2669,23 +2670,23 @@
         <v>0.99551462791969692</v>
       </c>
       <c r="I6" s="14">
-        <f t="shared" si="4"/>
-        <v>94272.696156477454</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>93465.49187412046</v>
       </c>
       <c r="J6" s="14">
-        <f t="shared" si="1"/>
-        <v>422.84811927516421</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>419.22750772397558</v>
       </c>
       <c r="K6" s="14">
-        <f t="shared" si="2"/>
-        <v>470306.36048419931</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>466279.39060129237</v>
       </c>
       <c r="L6" s="14">
-        <f>L7+K6</f>
-        <v>6496667.1655036304</v>
+        <f ca="1">L7+K6</f>
+        <v>6441039.8442234769</v>
       </c>
       <c r="M6" s="15">
-        <f t="shared" si="3"/>
+        <f t="shared" ca="1" si="2"/>
         <v>68.913560663632779</v>
       </c>
       <c r="O6" s="4"/>
@@ -2712,7 +2713,7 @@
         <v>2.5</v>
       </c>
       <c r="G7" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>3.5131047220755504E-3</v>
       </c>
       <c r="H7" s="12">
@@ -2720,24 +2721,24 @@
         <v>0.99648689527792444</v>
       </c>
       <c r="I7" s="14">
-        <f t="shared" si="4"/>
-        <v>93849.84803720229</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>93046.264366396485</v>
       </c>
       <c r="J7" s="14">
-        <f t="shared" si="1"/>
-        <v>329.70434430557361</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>326.88127071707277</v>
       </c>
       <c r="K7" s="14">
-        <f t="shared" si="2"/>
-        <v>468424.97932524752</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>464414.11865518976</v>
       </c>
       <c r="L7" s="14">
-        <f>L8+K7</f>
-        <v>6026360.8050194308</v>
+        <f ca="1">L8+K7</f>
+        <v>5974760.4536221847</v>
       </c>
       <c r="M7" s="15">
-        <f t="shared" si="3"/>
-        <v>64.212792359882869</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>64.212792359882854</v>
       </c>
       <c r="O7" s="4"/>
     </row>
@@ -2763,7 +2764,7 @@
         <v>2.5</v>
       </c>
       <c r="G8" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>5.0836296176954114E-3</v>
       </c>
       <c r="H8" s="12">
@@ -2771,24 +2772,24 @@
         <v>0.99491637038230463</v>
       </c>
       <c r="I8" s="14">
-        <f t="shared" si="4"/>
-        <v>93520.143692896716</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>92719.383095679412</v>
       </c>
       <c r="J8" s="14">
-        <f t="shared" si="1"/>
-        <v>475.42177232833637</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>471.3510020396352</v>
       </c>
       <c r="K8" s="14">
-        <f t="shared" si="2"/>
-        <v>466412.16403366276</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>462418.53797329799</v>
       </c>
       <c r="L8" s="14">
-        <f t="shared" ref="L8:L19" si="7">L9+K8</f>
-        <v>5557935.8256941829</v>
+        <f t="shared" ref="L8:L19" ca="1" si="7">L9+K8</f>
+        <v>5510346.3349669948</v>
       </c>
       <c r="M8" s="15">
-        <f t="shared" si="3"/>
-        <v>59.430360200743934</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>59.430360200743927</v>
       </c>
       <c r="O8" s="4"/>
     </row>
@@ -2814,7 +2815,7 @@
         <v>2.5</v>
       </c>
       <c r="G9" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>7.2779444124459487E-3</v>
       </c>
       <c r="H9" s="12">
@@ -2822,24 +2823,24 @@
         <v>0.992722055587554</v>
       </c>
       <c r="I9" s="14">
-        <f t="shared" si="4"/>
-        <v>93044.72192056838</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>92248.032093639777</v>
       </c>
       <c r="J9" s="14">
-        <f t="shared" si="1"/>
-        <v>677.17431400938949</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>671.37604973504494</v>
       </c>
       <c r="K9" s="14">
-        <f t="shared" si="2"/>
-        <v>463530.67381781846</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>459561.72034386126</v>
       </c>
       <c r="L9" s="14">
-        <f t="shared" si="7"/>
-        <v>5091523.6616605204</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>5047927.7969936971</v>
       </c>
       <c r="M9" s="15">
-        <f t="shared" si="3"/>
-        <v>54.721251851417406</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>54.721251851417399</v>
       </c>
       <c r="O9" s="4"/>
     </row>
@@ -2865,7 +2866,7 @@
         <v>2.5</v>
       </c>
       <c r="G10" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>9.4209292690003651E-3</v>
       </c>
       <c r="H10" s="12">
@@ -2873,24 +2874,24 @@
         <v>0.9905790707309996</v>
       </c>
       <c r="I10" s="14">
-        <f t="shared" si="4"/>
-        <v>92367.54760655899</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>91576.656043904732</v>
       </c>
       <c r="J10" s="14">
-        <f t="shared" si="1"/>
-        <v>870.188132752417</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>862.73719928121136</v>
       </c>
       <c r="K10" s="14">
-        <f t="shared" si="2"/>
-        <v>459662.26770091389</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>455726.43722132058</v>
       </c>
       <c r="L10" s="14">
-        <f t="shared" si="7"/>
-        <v>4627992.9878427023</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>4588366.0766498363</v>
       </c>
       <c r="M10" s="15">
-        <f t="shared" si="3"/>
-        <v>50.10410157857293</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>50.104101578572916</v>
       </c>
       <c r="O10" s="4"/>
     </row>
@@ -2916,7 +2917,7 @@
         <v>2.5</v>
       </c>
       <c r="G11" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>1.1667606804619542E-2</v>
       </c>
       <c r="H11" s="12">
@@ -2924,24 +2925,24 @@
         <v>0.98833239319538047</v>
       </c>
       <c r="I11" s="14">
-        <f t="shared" si="4"/>
-        <v>91497.359473806573</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>90713.91884462352</v>
       </c>
       <c r="J11" s="14">
-        <f t="shared" si="1"/>
-        <v>1067.5552140013024</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>1058.4143367852375</v>
       </c>
       <c r="K11" s="14">
-        <f t="shared" si="2"/>
-        <v>454817.90933402959</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>450923.55838115449</v>
       </c>
       <c r="L11" s="14">
-        <f t="shared" si="7"/>
-        <v>4168330.7201417885</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>4132639.6394285159</v>
       </c>
       <c r="M11" s="15">
-        <f t="shared" si="3"/>
-        <v>45.556841684978664</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>45.556841684978657</v>
       </c>
       <c r="O11" s="4"/>
     </row>
@@ -2975,23 +2976,23 @@
         <v>0.98572741873750258</v>
       </c>
       <c r="I12" s="14">
-        <f t="shared" si="4"/>
-        <v>90429.804259805271</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>89655.504507838283</v>
       </c>
       <c r="J12" s="14">
-        <f t="shared" si="1"/>
-        <v>1290.6667298498069</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>1279.6154737183242</v>
       </c>
       <c r="K12" s="14">
-        <f t="shared" si="2"/>
-        <v>448922.35447440186</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>445078.48385489557</v>
       </c>
       <c r="L12" s="14">
-        <f t="shared" si="7"/>
-        <v>3713512.8108077589</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>3681716.0810473613</v>
       </c>
       <c r="M12" s="15">
-        <f t="shared" si="3"/>
+        <f t="shared" ca="1" si="2"/>
         <v>41.065142639685675</v>
       </c>
       <c r="O12" s="4"/>
@@ -3026,23 +3027,23 @@
         <v>0.98199686794825947</v>
       </c>
       <c r="I13" s="14">
-        <f t="shared" si="4"/>
-        <v>89139.137529955464</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>88375.889034119959</v>
       </c>
       <c r="J13" s="14">
-        <f t="shared" ref="J13:J20" si="10">I13-I14</f>
-        <v>1604.7836639300513</v>
+        <f t="shared" ref="J13:J20" ca="1" si="10">I13-I14</f>
+        <v>1591.0428004712303</v>
       </c>
       <c r="K13" s="14">
-        <f t="shared" si="2"/>
-        <v>441683.72848995216</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>437901.83816942171</v>
       </c>
       <c r="L13" s="14">
-        <f t="shared" si="7"/>
-        <v>3264590.4563333569</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>3236637.5971924658</v>
       </c>
       <c r="M13" s="15">
-        <f t="shared" si="3"/>
+        <f t="shared" ca="1" si="2"/>
         <v>36.623536493566384</v>
       </c>
       <c r="O13" s="4"/>
@@ -3077,23 +3078,23 @@
         <v>0.97647247882648647</v>
       </c>
       <c r="I14" s="14">
-        <f t="shared" si="4"/>
-        <v>87534.353866025413</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>86784.846233648728</v>
       </c>
       <c r="J14" s="14">
-        <f t="shared" si="10"/>
-        <v>2059.4663639927458</v>
+        <f t="shared" ca="1" si="10"/>
+        <v>2041.8323073022912</v>
       </c>
       <c r="K14" s="14">
-        <f t="shared" ref="K14:K19" si="11">(B14*I15)+(F14*J14)</f>
-        <v>432523.10342014523</v>
+        <f t="shared" ref="K14:K19" ca="1" si="11">(B14*I15)+(F14*J14)</f>
+        <v>428819.65039998794</v>
       </c>
       <c r="L14" s="14">
-        <f t="shared" si="7"/>
-        <v>2822906.7278434047</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>2798735.7590230443</v>
       </c>
       <c r="M14" s="15">
-        <f t="shared" si="3"/>
+        <f t="shared" ca="1" si="2"/>
         <v>32.249129663582927</v>
       </c>
       <c r="O14" s="4"/>
@@ -3128,23 +3129,23 @@
         <v>0.96582443099525839</v>
       </c>
       <c r="I15" s="14">
-        <f t="shared" si="4"/>
-        <v>85474.887502032667</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>84743.013926346437</v>
       </c>
       <c r="J15" s="14">
-        <f t="shared" si="10"/>
-        <v>2921.1529159982456</v>
+        <f t="shared" ca="1" si="10"/>
+        <v>2896.1407201096299</v>
       </c>
       <c r="K15" s="14">
-        <f t="shared" si="11"/>
-        <v>420071.55522016773</v>
+        <f t="shared" ca="1" si="11"/>
+        <v>416474.71783145808</v>
       </c>
       <c r="L15" s="14">
-        <f t="shared" si="7"/>
-        <v>2390383.6244232594</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>2369916.1086230562</v>
       </c>
       <c r="M15" s="15">
-        <f t="shared" si="3"/>
+        <f t="shared" ca="1" si="2"/>
         <v>27.965917174987965</v>
       </c>
       <c r="O15" s="4"/>
@@ -3179,24 +3180,24 @@
         <v>0.95109899805886156</v>
       </c>
       <c r="I16" s="14">
-        <f t="shared" ref="I16:I21" si="12">I15*H15</f>
-        <v>82553.734586034421</v>
+        <f t="shared" ref="I16:I21" ca="1" si="12">I15*H15</f>
+        <v>81846.873206236807</v>
       </c>
       <c r="J16" s="14">
-        <f t="shared" si="10"/>
-        <v>4036.960335239899</v>
+        <f t="shared" ca="1" si="10"/>
+        <v>4002.3941055343021</v>
       </c>
       <c r="K16" s="14">
-        <f t="shared" si="11"/>
-        <v>402676.27209207241</v>
+        <f t="shared" ca="1" si="11"/>
+        <v>399228.38076734828</v>
       </c>
       <c r="L16" s="14">
-        <f t="shared" si="7"/>
-        <v>1970312.0692030918</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>1953441.3907915982</v>
       </c>
       <c r="M16" s="15">
-        <f t="shared" si="3"/>
-        <v>23.86702526643063</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>23.867025266430634</v>
       </c>
       <c r="O16" s="4"/>
     </row>
@@ -3230,24 +3231,24 @@
         <v>0.92436910744787204</v>
       </c>
       <c r="I17" s="14">
-        <f t="shared" si="12"/>
-        <v>78516.774250794522</v>
+        <f t="shared" ca="1" si="12"/>
+        <v>77844.479100702505</v>
       </c>
       <c r="J17" s="14">
-        <f t="shared" si="10"/>
-        <v>5938.2937169015349</v>
+        <f t="shared" ca="1" si="10"/>
+        <v>5887.4474346415955</v>
       </c>
       <c r="K17" s="14">
-        <f t="shared" si="11"/>
-        <v>377738.13696171879</v>
+        <f t="shared" ca="1" si="11"/>
+        <v>374503.77691690857</v>
       </c>
       <c r="L17" s="14">
-        <f t="shared" si="7"/>
-        <v>1567635.7971110193</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>1554213.01002425</v>
       </c>
       <c r="M17" s="15">
-        <f t="shared" si="3"/>
-        <v>19.965616418521627</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>19.965616418521634</v>
       </c>
       <c r="O17" s="4"/>
     </row>
@@ -3281,24 +3282,24 @@
         <v>0.8948905569592327</v>
       </c>
       <c r="I18" s="14">
-        <f t="shared" si="12"/>
-        <v>72578.480533892987</v>
+        <f t="shared" ca="1" si="12"/>
+        <v>71957.03166606091</v>
       </c>
       <c r="J18" s="14">
-        <f t="shared" si="10"/>
-        <v>7628.683665662662</v>
+        <f t="shared" ca="1" si="10"/>
+        <v>7563.3635212865192</v>
       </c>
       <c r="K18" s="14">
-        <f t="shared" si="11"/>
-        <v>343820.69350530824</v>
+        <f t="shared" ca="1" si="11"/>
+        <v>340876.74952708825</v>
       </c>
       <c r="L18" s="14">
-        <f t="shared" si="7"/>
-        <v>1189897.6601493005</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>1179709.2331073415</v>
       </c>
       <c r="M18" s="15">
-        <f t="shared" si="3"/>
-        <v>16.394634489401266</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>16.39463448940127</v>
       </c>
       <c r="O18" s="4"/>
     </row>
@@ -3332,23 +3333,23 @@
         <v>0.84822817151744057</v>
       </c>
       <c r="I19" s="14">
-        <f t="shared" si="12"/>
-        <v>64949.796868230325</v>
+        <f t="shared" ca="1" si="12"/>
+        <v>64393.66814477439</v>
       </c>
       <c r="J19" s="14">
-        <f t="shared" si="10"/>
-        <v>9857.54943026213</v>
+        <f t="shared" ca="1" si="10"/>
+        <v>9773.1447570315504</v>
       </c>
       <c r="K19" s="14">
-        <f t="shared" si="11"/>
-        <v>300105.11076549633</v>
+        <f t="shared" ca="1" si="11"/>
+        <v>297535.47883129306</v>
       </c>
       <c r="L19" s="14">
-        <f t="shared" si="7"/>
-        <v>846076.96664399235</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>838832.4835802532</v>
       </c>
       <c r="M19" s="15">
-        <f t="shared" si="3"/>
+        <f t="shared" ca="1" si="2"/>
         <v>13.026629911722544</v>
       </c>
       <c r="O19" s="4"/>
@@ -3383,23 +3384,23 @@
         <v>0.74846939330339179</v>
       </c>
       <c r="I20" s="14">
-        <f t="shared" si="12"/>
-        <v>55092.247437968195</v>
+        <f t="shared" ca="1" si="12"/>
+        <v>54620.52338774284</v>
       </c>
       <c r="J20" s="14">
-        <f t="shared" si="10"/>
-        <v>13857.386422351796</v>
+        <f t="shared" ca="1" si="10"/>
+        <v>13738.733385805237</v>
       </c>
       <c r="K20" s="14">
-        <f>(B20*I21)+(F20*J20)</f>
-        <v>240817.77113396148</v>
+        <f ca="1">(B20*I21)+(F20*J20)</f>
+        <v>238755.7834742011</v>
       </c>
       <c r="L20" s="14">
-        <f>L21+K20</f>
-        <v>545971.85587849608</v>
+        <f ca="1">L21+K20</f>
+        <v>541297.00474896014</v>
       </c>
       <c r="M20" s="15">
-        <f t="shared" si="3"/>
+        <f t="shared" ca="1" si="2"/>
         <v>9.9101394709526041</v>
       </c>
       <c r="O20" s="4"/>
@@ -3434,23 +3435,23 @@
         <v>0.59597541400775167</v>
       </c>
       <c r="I21" s="14">
-        <f t="shared" si="12"/>
-        <v>41234.8610156164</v>
+        <f t="shared" ca="1" si="12"/>
+        <v>40881.790001937603</v>
       </c>
       <c r="J21" s="14">
-        <f>I21-I22</f>
-        <v>16659.897650282317</v>
+        <f ca="1">I21-I22</f>
+        <v>16517.248280154876</v>
       </c>
       <c r="K21" s="14">
-        <f>(B21*I22)+(F21*J21)</f>
-        <v>164524.56095237623</v>
+        <f ca="1">(B21*I22)+(F21*J21)</f>
+        <v>163115.82930930084</v>
       </c>
       <c r="L21" s="14">
-        <f>L22+K21</f>
-        <v>305154.08474453463</v>
+        <f ca="1">L22+K21</f>
+        <v>302541.22127475904</v>
       </c>
       <c r="M21" s="15">
-        <f t="shared" si="3"/>
+        <f t="shared" ca="1" si="2"/>
         <v>7.4003907671464484</v>
       </c>
       <c r="O21" s="4"/>
@@ -3484,23 +3485,23 @@
         <v>0</v>
       </c>
       <c r="I22" s="14">
-        <f>I21*H21</f>
-        <v>24574.963365334082</v>
+        <f ca="1">I21*H21</f>
+        <v>24364.541721782727</v>
       </c>
       <c r="J22" s="14">
-        <f>I22-I23</f>
-        <v>24574.963365334082</v>
+        <f ca="1">I22-I23</f>
+        <v>24364.541721782727</v>
       </c>
       <c r="K22" s="14">
-        <f>I22/E22</f>
-        <v>140629.5237921584</v>
+        <f ca="1">I22/E22</f>
+        <v>139425.3919654582</v>
       </c>
       <c r="L22" s="14">
-        <f>K22</f>
-        <v>140629.5237921584</v>
+        <f ca="1">K22</f>
+        <v>139425.3919654582</v>
       </c>
       <c r="M22" s="15">
-        <f t="shared" si="3"/>
+        <f t="shared" ca="1" si="2"/>
         <v>5.7224713502740405</v>
       </c>
       <c r="O22" s="4"/>
@@ -4025,7 +4026,7 @@
         <f t="shared" si="2"/>
         <v>4270361.2785446141</v>
       </c>
-      <c r="M12" s="32">
+      <c r="M12" s="15">
         <f t="shared" si="6"/>
         <v>45.545382362087082</v>
       </c>
@@ -4611,8 +4612,8 @@
         <v>0</v>
       </c>
       <c r="C3" s="27">
-        <f>'tabla mortalidad 1998'!E4</f>
-        <v>3.6853451840742804E-2</v>
+        <f ca="1">'tabla mortalidad 1998'!E4</f>
+        <v>4.5645260778884852E-2</v>
       </c>
       <c r="D3" s="27">
         <f>'tabla mortalidad 2018'!E4</f>
@@ -4623,7 +4624,7 @@
       </c>
       <c r="G3" s="27">
         <f>'tabla mortalidad 1998'!G4</f>
-        <v>3.574197216833902E-2</v>
+        <v>4.3999999999999997E-2</v>
       </c>
       <c r="H3" s="27">
         <f>'tabla mortalidad 2018'!G4</f>
@@ -4645,7 +4646,7 @@
       </c>
       <c r="O3" s="1">
         <f>'tabla mortalidad 1998'!J4</f>
-        <v>3574.197216833898</v>
+        <v>4400</v>
       </c>
       <c r="P3" s="1">
         <f>'tabla mortalidad 2018'!J4</f>
@@ -4655,8 +4656,8 @@
         <v>0</v>
       </c>
       <c r="S3" s="28">
-        <f>'tabla mortalidad 1998'!M4</f>
-        <v>69.738985814585519</v>
+        <f ca="1">'tabla mortalidad 1998'!M4</f>
+        <v>69.143981836870424</v>
       </c>
       <c r="T3" s="28">
         <f>'tabla mortalidad 2018'!M4</f>
@@ -4679,8 +4680,8 @@
         <v>1</v>
       </c>
       <c r="G4" s="27">
-        <f>'tabla mortalidad 1998'!G5</f>
-        <v>2.2329154277619726E-2</v>
+        <f ca="1">'tabla mortalidad 1998'!G5</f>
+        <v>2.2327490856480562E-2</v>
       </c>
       <c r="H4" s="27">
         <f>'tabla mortalidad 2018'!G5</f>
@@ -4691,7 +4692,7 @@
       </c>
       <c r="K4" s="1">
         <f>'tabla mortalidad 1998'!I5</f>
-        <v>96425.802783166102</v>
+        <v>95600</v>
       </c>
       <c r="L4" s="1">
         <f>'tabla mortalidad 2018'!I5</f>
@@ -4701,8 +4702,8 @@
         <v>1</v>
       </c>
       <c r="O4" s="1">
-        <f>'tabla mortalidad 1998'!J5</f>
-        <v>2153.1066266886482</v>
+        <f ca="1">'tabla mortalidad 1998'!J5</f>
+        <v>2134.5081258795399</v>
       </c>
       <c r="P4" s="1">
         <f>'tabla mortalidad 2018'!J5</f>
@@ -4712,8 +4713,8 @@
         <v>1</v>
       </c>
       <c r="S4" s="28">
-        <f>'tabla mortalidad 1998'!M5</f>
-        <v>71.318198319521343</v>
+        <f ca="1">'tabla mortalidad 1998'!M5</f>
+        <v>71.318019184877059</v>
       </c>
       <c r="T4" s="28">
         <f>'tabla mortalidad 2018'!M5</f>
@@ -4747,8 +4748,8 @@
         <v>5</v>
       </c>
       <c r="K5" s="1">
-        <f>'tabla mortalidad 1998'!I6</f>
-        <v>94272.696156477454</v>
+        <f ca="1">'tabla mortalidad 1998'!I6</f>
+        <v>93465.49187412046</v>
       </c>
       <c r="L5" s="1">
         <f>'tabla mortalidad 2018'!I6</f>
@@ -4758,8 +4759,8 @@
         <v>5</v>
       </c>
       <c r="O5" s="1">
-        <f>'tabla mortalidad 1998'!J6</f>
-        <v>422.84811927516421</v>
+        <f ca="1">'tabla mortalidad 1998'!J6</f>
+        <v>419.22750772397558</v>
       </c>
       <c r="P5" s="1">
         <f>'tabla mortalidad 2018'!J6</f>
@@ -4769,7 +4770,7 @@
         <v>5</v>
       </c>
       <c r="S5" s="28">
-        <f>'tabla mortalidad 1998'!M6</f>
+        <f ca="1">'tabla mortalidad 1998'!M6</f>
         <v>68.913560663632779</v>
       </c>
       <c r="T5" s="28">
@@ -4804,8 +4805,8 @@
         <v>10</v>
       </c>
       <c r="K6" s="1">
-        <f>'tabla mortalidad 1998'!I7</f>
-        <v>93849.84803720229</v>
+        <f ca="1">'tabla mortalidad 1998'!I7</f>
+        <v>93046.264366396485</v>
       </c>
       <c r="L6" s="1">
         <f>'tabla mortalidad 2018'!I7</f>
@@ -4815,8 +4816,8 @@
         <v>10</v>
       </c>
       <c r="O6" s="1">
-        <f>'tabla mortalidad 1998'!J7</f>
-        <v>329.70434430557361</v>
+        <f ca="1">'tabla mortalidad 1998'!J7</f>
+        <v>326.88127071707277</v>
       </c>
       <c r="P6" s="1">
         <f>'tabla mortalidad 2018'!J7</f>
@@ -4826,8 +4827,8 @@
         <v>10</v>
       </c>
       <c r="S6" s="28">
-        <f>'tabla mortalidad 1998'!M7</f>
-        <v>64.212792359882869</v>
+        <f ca="1">'tabla mortalidad 1998'!M7</f>
+        <v>64.212792359882854</v>
       </c>
       <c r="T6" s="28">
         <f>'tabla mortalidad 2018'!M7</f>
@@ -4861,8 +4862,8 @@
         <v>15</v>
       </c>
       <c r="K7" s="1">
-        <f>'tabla mortalidad 1998'!I8</f>
-        <v>93520.143692896716</v>
+        <f ca="1">'tabla mortalidad 1998'!I8</f>
+        <v>92719.383095679412</v>
       </c>
       <c r="L7" s="1">
         <f>'tabla mortalidad 2018'!I8</f>
@@ -4872,8 +4873,8 @@
         <v>15</v>
       </c>
       <c r="O7" s="1">
-        <f>'tabla mortalidad 1998'!J8</f>
-        <v>475.42177232833637</v>
+        <f ca="1">'tabla mortalidad 1998'!J8</f>
+        <v>471.3510020396352</v>
       </c>
       <c r="P7" s="1">
         <f>'tabla mortalidad 2018'!J8</f>
@@ -4883,8 +4884,8 @@
         <v>15</v>
       </c>
       <c r="S7" s="28">
-        <f>'tabla mortalidad 1998'!M8</f>
-        <v>59.430360200743934</v>
+        <f ca="1">'tabla mortalidad 1998'!M8</f>
+        <v>59.430360200743927</v>
       </c>
       <c r="T7" s="28">
         <f>'tabla mortalidad 2018'!M8</f>
@@ -4918,8 +4919,8 @@
         <v>20</v>
       </c>
       <c r="K8" s="1">
-        <f>'tabla mortalidad 1998'!I9</f>
-        <v>93044.72192056838</v>
+        <f ca="1">'tabla mortalidad 1998'!I9</f>
+        <v>92248.032093639777</v>
       </c>
       <c r="L8" s="1">
         <f>'tabla mortalidad 2018'!I9</f>
@@ -4929,8 +4930,8 @@
         <v>20</v>
       </c>
       <c r="O8" s="1">
-        <f>'tabla mortalidad 1998'!J9</f>
-        <v>677.17431400938949</v>
+        <f ca="1">'tabla mortalidad 1998'!J9</f>
+        <v>671.37604973504494</v>
       </c>
       <c r="P8" s="1">
         <f>'tabla mortalidad 2018'!J9</f>
@@ -4940,8 +4941,8 @@
         <v>20</v>
       </c>
       <c r="S8" s="28">
-        <f>'tabla mortalidad 1998'!M9</f>
-        <v>54.721251851417406</v>
+        <f ca="1">'tabla mortalidad 1998'!M9</f>
+        <v>54.721251851417399</v>
       </c>
       <c r="T8" s="28">
         <f>'tabla mortalidad 2018'!M9</f>
@@ -4975,8 +4976,8 @@
         <v>25</v>
       </c>
       <c r="K9" s="1">
-        <f>'tabla mortalidad 1998'!I10</f>
-        <v>92367.54760655899</v>
+        <f ca="1">'tabla mortalidad 1998'!I10</f>
+        <v>91576.656043904732</v>
       </c>
       <c r="L9" s="1">
         <f>'tabla mortalidad 2018'!I10</f>
@@ -4986,8 +4987,8 @@
         <v>25</v>
       </c>
       <c r="O9" s="1">
-        <f>'tabla mortalidad 1998'!J10</f>
-        <v>870.188132752417</v>
+        <f ca="1">'tabla mortalidad 1998'!J10</f>
+        <v>862.73719928121136</v>
       </c>
       <c r="P9" s="1">
         <f>'tabla mortalidad 2018'!J10</f>
@@ -4997,8 +4998,8 @@
         <v>25</v>
       </c>
       <c r="S9" s="28">
-        <f>'tabla mortalidad 1998'!M10</f>
-        <v>50.10410157857293</v>
+        <f ca="1">'tabla mortalidad 1998'!M10</f>
+        <v>50.104101578572916</v>
       </c>
       <c r="T9" s="28">
         <f>'tabla mortalidad 2018'!M10</f>
@@ -5032,8 +5033,8 @@
         <v>30</v>
       </c>
       <c r="K10" s="1">
-        <f>'tabla mortalidad 1998'!I11</f>
-        <v>91497.359473806573</v>
+        <f ca="1">'tabla mortalidad 1998'!I11</f>
+        <v>90713.91884462352</v>
       </c>
       <c r="L10" s="1">
         <f>'tabla mortalidad 2018'!I11</f>
@@ -5043,8 +5044,8 @@
         <v>30</v>
       </c>
       <c r="O10" s="1">
-        <f>'tabla mortalidad 1998'!J11</f>
-        <v>1067.5552140013024</v>
+        <f ca="1">'tabla mortalidad 1998'!J11</f>
+        <v>1058.4143367852375</v>
       </c>
       <c r="P10" s="1">
         <f>'tabla mortalidad 2018'!J11</f>
@@ -5054,8 +5055,8 @@
         <v>30</v>
       </c>
       <c r="S10" s="28">
-        <f>'tabla mortalidad 1998'!M11</f>
-        <v>45.556841684978664</v>
+        <f ca="1">'tabla mortalidad 1998'!M11</f>
+        <v>45.556841684978657</v>
       </c>
       <c r="T10" s="28">
         <f>'tabla mortalidad 2018'!M11</f>
@@ -5089,8 +5090,8 @@
         <v>35</v>
       </c>
       <c r="K11" s="1">
-        <f>'tabla mortalidad 1998'!I12</f>
-        <v>90429.804259805271</v>
+        <f ca="1">'tabla mortalidad 1998'!I12</f>
+        <v>89655.504507838283</v>
       </c>
       <c r="L11" s="1">
         <f>'tabla mortalidad 2018'!I12</f>
@@ -5100,8 +5101,8 @@
         <v>35</v>
       </c>
       <c r="O11" s="1">
-        <f>'tabla mortalidad 1998'!J12</f>
-        <v>1290.6667298498069</v>
+        <f ca="1">'tabla mortalidad 1998'!J12</f>
+        <v>1279.6154737183242</v>
       </c>
       <c r="P11" s="1">
         <f>'tabla mortalidad 2018'!J12</f>
@@ -5111,7 +5112,7 @@
         <v>35</v>
       </c>
       <c r="S11" s="28">
-        <f>'tabla mortalidad 1998'!M12</f>
+        <f ca="1">'tabla mortalidad 1998'!M12</f>
         <v>41.065142639685675</v>
       </c>
       <c r="T11" s="28">
@@ -5146,8 +5147,8 @@
         <v>40</v>
       </c>
       <c r="K12" s="1">
-        <f>'tabla mortalidad 1998'!I13</f>
-        <v>89139.137529955464</v>
+        <f ca="1">'tabla mortalidad 1998'!I13</f>
+        <v>88375.889034119959</v>
       </c>
       <c r="L12" s="1">
         <f>'tabla mortalidad 2018'!I13</f>
@@ -5157,8 +5158,8 @@
         <v>40</v>
       </c>
       <c r="O12" s="1">
-        <f>'tabla mortalidad 1998'!J13</f>
-        <v>1604.7836639300513</v>
+        <f ca="1">'tabla mortalidad 1998'!J13</f>
+        <v>1591.0428004712303</v>
       </c>
       <c r="P12" s="1">
         <f>'tabla mortalidad 2018'!J13</f>
@@ -5168,7 +5169,7 @@
         <v>40</v>
       </c>
       <c r="S12" s="28">
-        <f>'tabla mortalidad 1998'!M13</f>
+        <f ca="1">'tabla mortalidad 1998'!M13</f>
         <v>36.623536493566384</v>
       </c>
       <c r="T12" s="28">
@@ -5203,8 +5204,8 @@
         <v>45</v>
       </c>
       <c r="K13" s="1">
-        <f>'tabla mortalidad 1998'!I14</f>
-        <v>87534.353866025413</v>
+        <f ca="1">'tabla mortalidad 1998'!I14</f>
+        <v>86784.846233648728</v>
       </c>
       <c r="L13" s="1">
         <f>'tabla mortalidad 2018'!I14</f>
@@ -5214,8 +5215,8 @@
         <v>45</v>
       </c>
       <c r="O13" s="1">
-        <f>'tabla mortalidad 1998'!J14</f>
-        <v>2059.4663639927458</v>
+        <f ca="1">'tabla mortalidad 1998'!J14</f>
+        <v>2041.8323073022912</v>
       </c>
       <c r="P13" s="1">
         <f>'tabla mortalidad 2018'!J14</f>
@@ -5225,7 +5226,7 @@
         <v>45</v>
       </c>
       <c r="S13" s="28">
-        <f>'tabla mortalidad 1998'!M14</f>
+        <f ca="1">'tabla mortalidad 1998'!M14</f>
         <v>32.249129663582927</v>
       </c>
       <c r="T13" s="28">
@@ -5260,8 +5261,8 @@
         <v>50</v>
       </c>
       <c r="K14" s="1">
-        <f>'tabla mortalidad 1998'!I15</f>
-        <v>85474.887502032667</v>
+        <f ca="1">'tabla mortalidad 1998'!I15</f>
+        <v>84743.013926346437</v>
       </c>
       <c r="L14" s="1">
         <f>'tabla mortalidad 2018'!I15</f>
@@ -5271,8 +5272,8 @@
         <v>50</v>
       </c>
       <c r="O14" s="1">
-        <f>'tabla mortalidad 1998'!J15</f>
-        <v>2921.1529159982456</v>
+        <f ca="1">'tabla mortalidad 1998'!J15</f>
+        <v>2896.1407201096299</v>
       </c>
       <c r="P14" s="1">
         <f>'tabla mortalidad 2018'!J15</f>
@@ -5282,7 +5283,7 @@
         <v>50</v>
       </c>
       <c r="S14" s="28">
-        <f>'tabla mortalidad 1998'!M15</f>
+        <f ca="1">'tabla mortalidad 1998'!M15</f>
         <v>27.965917174987965</v>
       </c>
       <c r="T14" s="28">
@@ -5317,8 +5318,8 @@
         <v>55</v>
       </c>
       <c r="K15" s="1">
-        <f>'tabla mortalidad 1998'!I16</f>
-        <v>82553.734586034421</v>
+        <f ca="1">'tabla mortalidad 1998'!I16</f>
+        <v>81846.873206236807</v>
       </c>
       <c r="L15" s="1">
         <f>'tabla mortalidad 2018'!I16</f>
@@ -5328,8 +5329,8 @@
         <v>55</v>
       </c>
       <c r="O15" s="1">
-        <f>'tabla mortalidad 1998'!J16</f>
-        <v>4036.960335239899</v>
+        <f ca="1">'tabla mortalidad 1998'!J16</f>
+        <v>4002.3941055343021</v>
       </c>
       <c r="P15" s="1">
         <f>'tabla mortalidad 2018'!J16</f>
@@ -5339,8 +5340,8 @@
         <v>55</v>
       </c>
       <c r="S15" s="28">
-        <f>'tabla mortalidad 1998'!M16</f>
-        <v>23.86702526643063</v>
+        <f ca="1">'tabla mortalidad 1998'!M16</f>
+        <v>23.867025266430634</v>
       </c>
       <c r="T15" s="28">
         <f>'tabla mortalidad 2018'!M16</f>
@@ -5374,8 +5375,8 @@
         <v>60</v>
       </c>
       <c r="K16" s="1">
-        <f>'tabla mortalidad 1998'!I17</f>
-        <v>78516.774250794522</v>
+        <f ca="1">'tabla mortalidad 1998'!I17</f>
+        <v>77844.479100702505</v>
       </c>
       <c r="L16" s="1">
         <f>'tabla mortalidad 2018'!I17</f>
@@ -5385,8 +5386,8 @@
         <v>60</v>
       </c>
       <c r="O16" s="1">
-        <f>'tabla mortalidad 1998'!J17</f>
-        <v>5938.2937169015349</v>
+        <f ca="1">'tabla mortalidad 1998'!J17</f>
+        <v>5887.4474346415955</v>
       </c>
       <c r="P16" s="1">
         <f>'tabla mortalidad 2018'!J17</f>
@@ -5396,8 +5397,8 @@
         <v>60</v>
       </c>
       <c r="S16" s="28">
-        <f>'tabla mortalidad 1998'!M17</f>
-        <v>19.965616418521627</v>
+        <f ca="1">'tabla mortalidad 1998'!M17</f>
+        <v>19.965616418521634</v>
       </c>
       <c r="T16" s="28">
         <f>'tabla mortalidad 2018'!M17</f>
@@ -5431,8 +5432,8 @@
         <v>65</v>
       </c>
       <c r="K17" s="1">
-        <f>'tabla mortalidad 1998'!I18</f>
-        <v>72578.480533892987</v>
+        <f ca="1">'tabla mortalidad 1998'!I18</f>
+        <v>71957.03166606091</v>
       </c>
       <c r="L17" s="1">
         <f>'tabla mortalidad 2018'!I18</f>
@@ -5442,8 +5443,8 @@
         <v>65</v>
       </c>
       <c r="O17" s="1">
-        <f>'tabla mortalidad 1998'!J18</f>
-        <v>7628.683665662662</v>
+        <f ca="1">'tabla mortalidad 1998'!J18</f>
+        <v>7563.3635212865192</v>
       </c>
       <c r="P17" s="1">
         <f>'tabla mortalidad 2018'!J18</f>
@@ -5453,8 +5454,8 @@
         <v>65</v>
       </c>
       <c r="S17" s="28">
-        <f>'tabla mortalidad 1998'!M18</f>
-        <v>16.394634489401266</v>
+        <f ca="1">'tabla mortalidad 1998'!M18</f>
+        <v>16.39463448940127</v>
       </c>
       <c r="T17" s="28">
         <f>'tabla mortalidad 2018'!M18</f>
@@ -5488,8 +5489,8 @@
         <v>70</v>
       </c>
       <c r="K18" s="1">
-        <f>'tabla mortalidad 1998'!I19</f>
-        <v>64949.796868230325</v>
+        <f ca="1">'tabla mortalidad 1998'!I19</f>
+        <v>64393.66814477439</v>
       </c>
       <c r="L18" s="1">
         <f>'tabla mortalidad 2018'!I19</f>
@@ -5499,8 +5500,8 @@
         <v>70</v>
       </c>
       <c r="O18" s="1">
-        <f>'tabla mortalidad 1998'!J19</f>
-        <v>9857.54943026213</v>
+        <f ca="1">'tabla mortalidad 1998'!J19</f>
+        <v>9773.1447570315504</v>
       </c>
       <c r="P18" s="1">
         <f>'tabla mortalidad 2018'!J19</f>
@@ -5510,7 +5511,7 @@
         <v>70</v>
       </c>
       <c r="S18" s="28">
-        <f>'tabla mortalidad 1998'!M19</f>
+        <f ca="1">'tabla mortalidad 1998'!M19</f>
         <v>13.026629911722544</v>
       </c>
       <c r="T18" s="28">
@@ -5545,8 +5546,8 @@
         <v>75</v>
       </c>
       <c r="K19" s="1">
-        <f>'tabla mortalidad 1998'!I20</f>
-        <v>55092.247437968195</v>
+        <f ca="1">'tabla mortalidad 1998'!I20</f>
+        <v>54620.52338774284</v>
       </c>
       <c r="L19" s="1">
         <f>'tabla mortalidad 2018'!I20</f>
@@ -5556,8 +5557,8 @@
         <v>75</v>
       </c>
       <c r="O19" s="1">
-        <f>'tabla mortalidad 1998'!J20</f>
-        <v>13857.386422351796</v>
+        <f ca="1">'tabla mortalidad 1998'!J20</f>
+        <v>13738.733385805237</v>
       </c>
       <c r="P19" s="1">
         <f>'tabla mortalidad 2018'!J20</f>
@@ -5567,7 +5568,7 @@
         <v>75</v>
       </c>
       <c r="S19" s="28">
-        <f>'tabla mortalidad 1998'!M20</f>
+        <f ca="1">'tabla mortalidad 1998'!M20</f>
         <v>9.9101394709526041</v>
       </c>
       <c r="T19" s="28">
@@ -5602,8 +5603,8 @@
         <v>80</v>
       </c>
       <c r="K20" s="1">
-        <f>'tabla mortalidad 1998'!I21</f>
-        <v>41234.8610156164</v>
+        <f ca="1">'tabla mortalidad 1998'!I21</f>
+        <v>40881.790001937603</v>
       </c>
       <c r="L20" s="1">
         <f>'tabla mortalidad 2018'!I21</f>
@@ -5613,8 +5614,8 @@
         <v>80</v>
       </c>
       <c r="O20" s="1">
-        <f>'tabla mortalidad 1998'!J21</f>
-        <v>16659.897650282317</v>
+        <f ca="1">'tabla mortalidad 1998'!J21</f>
+        <v>16517.248280154876</v>
       </c>
       <c r="P20" s="1">
         <f>'tabla mortalidad 2018'!J21</f>
@@ -5624,7 +5625,7 @@
         <v>80</v>
       </c>
       <c r="S20" s="28">
-        <f>'tabla mortalidad 1998'!M21</f>
+        <f ca="1">'tabla mortalidad 1998'!M21</f>
         <v>7.4003907671464484</v>
       </c>
       <c r="T20" s="28">
@@ -5659,8 +5660,8 @@
         <v>13</v>
       </c>
       <c r="K21" s="1">
-        <f>'tabla mortalidad 1998'!I22</f>
-        <v>24574.963365334082</v>
+        <f ca="1">'tabla mortalidad 1998'!I22</f>
+        <v>24364.541721782727</v>
       </c>
       <c r="L21" s="1">
         <f>'tabla mortalidad 2018'!I22</f>
@@ -5670,8 +5671,8 @@
         <v>13</v>
       </c>
       <c r="O21" s="1">
-        <f>'tabla mortalidad 1998'!J22</f>
-        <v>24574.963365334082</v>
+        <f ca="1">'tabla mortalidad 1998'!J22</f>
+        <v>24364.541721782727</v>
       </c>
       <c r="P21" s="1">
         <f>'tabla mortalidad 2018'!J22</f>
@@ -5681,7 +5682,7 @@
         <v>13</v>
       </c>
       <c r="S21" s="28">
-        <f>'tabla mortalidad 1998'!M22</f>
+        <f ca="1">'tabla mortalidad 1998'!M22</f>
         <v>5.7224713502740405</v>
       </c>
       <c r="T21" s="28">

</xml_diff>